<commit_message>
Movement upgrades in, need to find cost/stat table values...
</commit_message>
<xml_diff>
--- a/_docs/Regolith Upgrades.xlsx
+++ b/_docs/Regolith Upgrades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\IwEngine\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCFB903-9FEF-4EC8-814C-6A95B59F9641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F32977A-EF17-45B5-8271-FA06EFD1066D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-3770" windowWidth="38620" windowHeight="21820" xr2:uid="{155C16C2-EBE6-4459-A987-D2622056FA3E}"/>
+    <workbookView xWindow="3915" yWindow="2625" windowWidth="21540" windowHeight="15105" xr2:uid="{155C16C2-EBE6-4459-A987-D2622056FA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Moves</t>
   </si>
@@ -185,6 +185,15 @@
 Speed
 Damage to cells hit
 I frames</t>
+  </si>
+  <si>
+    <t>Number Bought</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -240,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,11 +266,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -295,6 +333,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85457940-B7D7-4377-BF76-11EE28B1EC99}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +677,10 @@
     <col min="7" max="7" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="10" max="10" width="9.140625" style="15"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -809,9 +864,381 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>10</v>
+      </c>
+      <c r="M21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f>L21+10</f>
+        <v>20</v>
+      </c>
+      <c r="M22">
+        <f>M21*1.1</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:L36" si="0">L22+10</f>
+        <v>30</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M36" si="1">M22*1.1</f>
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>1464.1000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>1610.5100000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>1771.5610000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>1948.7171000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="1"/>
+        <v>2143.5888100000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="1"/>
+        <v>2357.9476910000008</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>2593.7424601000012</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>11</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>2853.1167061100014</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>12</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>3138.4283767210018</v>
+      </c>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>13</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>3452.2712143931021</v>
+      </c>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>14</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>3797.4983358324125</v>
+      </c>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>15</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>4177.248169415654</v>
+      </c>
+    </row>
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>16</v>
+      </c>
+      <c r="L37">
+        <f t="shared" ref="L37:L46" si="2">L36+10</f>
+        <v>170</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ref="M37:M46" si="3">M36*1.1</f>
+        <v>4594.9729863572202</v>
+      </c>
+    </row>
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>17</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="3"/>
+        <v>5054.4702849929427</v>
+      </c>
+    </row>
+    <row r="39" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>18</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="3"/>
+        <v>5559.9173134922376</v>
+      </c>
+    </row>
+    <row r="40" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>19</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="3"/>
+        <v>6115.9090448414618</v>
+      </c>
+    </row>
+    <row r="41" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>20</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="3"/>
+        <v>6727.4999493256082</v>
+      </c>
+    </row>
+    <row r="42" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <v>21</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="3"/>
+        <v>7400.2499442581693</v>
+      </c>
+    </row>
+    <row r="43" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>22</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="3"/>
+        <v>8140.2749386839869</v>
+      </c>
+    </row>
+    <row r="44" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>23</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="3"/>
+        <v>8954.3024325523857</v>
+      </c>
+    </row>
+    <row r="45" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>24</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="3"/>
+        <v>9849.7326758076251</v>
+      </c>
+    </row>
+    <row r="46" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>25</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="2"/>
+        <v>260</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="3"/>
+        <v>10834.705943388388</v>
+      </c>
+    </row>
+    <row r="47" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>26</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ref="L47:L62" si="4">L46+10</f>
+        <v>270</v>
+      </c>
+      <c r="M47">
+        <f t="shared" ref="M47:M62" si="5">M46*1.1</f>
+        <v>11918.176537727228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>